<commit_message>
Add body fat percentage and exercise type to example dataset
</commit_message>
<xml_diff>
--- a/data/raw-data/exampledata2.xlsx
+++ b/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE544BE-E0CE-4940-AC05-EB4F40C1D1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E368943E-8104-DF4D-A4F0-2FEC2388D8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34560" yWindow="-5620" windowWidth="26780" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34560" yWindow="-5620" windowWidth="26780" windowHeight="20140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -78,6 +78,27 @@
   </si>
   <si>
     <t>Exercise_type</t>
+  </si>
+  <si>
+    <t>body fat percentage of individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type of exercise an individual perform </t>
+  </si>
+  <si>
+    <t>none/cardio/strength/mixed</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>cardio</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -121,9 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -422,10 +447,10 @@
       <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -439,6 +464,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -450,6 +481,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -461,6 +498,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -472,6 +515,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -483,6 +532,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -494,6 +549,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -505,6 +566,12 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -516,6 +583,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -527,6 +600,12 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -538,6 +617,12 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -546,6 +631,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -557,6 +648,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -568,6 +665,12 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14">
+        <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -578,6 +681,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -587,10 +696,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,10 +721,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
@@ -623,10 +732,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
@@ -634,14 +743,36 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>